<commit_message>
Uploaded the daily files
</commit_message>
<xml_diff>
--- a/files/Matières/EPS/T1/Récup des temps.xlsx
+++ b/files/Matières/EPS/T1/Récup des temps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\EPS\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69862183-DA4C-4CC5-87CC-A02A25EC87A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A32C0A3-ABAE-4B38-8145-01233A24F352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{57035DCE-7893-496B-BF95-86A9CDE9C012}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>Temps Graçon</t>
-  </si>
-  <si>
     <t>Temps Fille</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>HS', "7'99",  "0'00" Pas:0'01</t>
+  </si>
+  <si>
+    <t>Temps Garçon</t>
   </si>
 </sst>
 </file>
@@ -232,24 +232,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -264,6 +246,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,7 +592,7 @@
   <dimension ref="C1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -614,65 +614,65 @@
   <sheetData>
     <row r="1" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="K2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="K2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14"/>
     </row>
     <row r="3" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="K3" s="8" t="s">
+      <c r="H3" s="4"/>
+      <c r="K3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="10"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="17"/>
-      <c r="K4" s="7" t="s">
-        <v>14</v>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -680,149 +680,149 @@
       <c r="P4" s="17"/>
     </row>
     <row r="5" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="K5" s="8" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="K5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
     </row>
     <row r="6" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
-      <c r="K6" s="8" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="K6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="4"/>
     </row>
     <row r="7" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
-      <c r="K7" s="8" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="K7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C8" s="7"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
     </row>
     <row r="9" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="11">
+      <c r="E9" s="3"/>
+      <c r="F9" s="5">
         <v>2</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="12">
+      <c r="G9" s="3"/>
+      <c r="H9" s="6">
         <v>4</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="5">
         <v>0</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="11">
+      <c r="M9" s="3"/>
+      <c r="N9" s="5">
         <v>2</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="12">
+      <c r="O9" s="3"/>
+      <c r="P9" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="7">
         <v>0</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="13">
+      <c r="E10" s="3"/>
+      <c r="F10" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="14">
+      <c r="G10" s="3"/>
+      <c r="H10" s="8">
         <v>2</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="7">
         <v>0</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="13">
+      <c r="M10" s="3"/>
+      <c r="N10" s="7">
         <v>1</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="14">
+      <c r="O10" s="3"/>
+      <c r="P10" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
-      <c r="K11" s="7" t="s">
-        <v>14</v>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
@@ -830,130 +830,130 @@
       <c r="P11" s="17"/>
     </row>
     <row r="12" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="K12" s="8" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="K12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="10"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="4"/>
     </row>
     <row r="13" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="K13" s="8" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+      <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="4"/>
     </row>
     <row r="14" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="K14" s="8" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="K14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="6"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
     </row>
     <row r="16" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="7">
         <v>0</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="13">
+      <c r="E16" s="3"/>
+      <c r="F16" s="7">
         <v>2</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="14">
+      <c r="G16" s="3"/>
+      <c r="H16" s="8">
         <v>4</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="7">
         <v>0</v>
       </c>
-      <c r="M16" s="9"/>
-      <c r="N16" s="13">
+      <c r="M16" s="3"/>
+      <c r="N16" s="7">
         <v>2</v>
       </c>
-      <c r="O16" s="9"/>
-      <c r="P16" s="14">
+      <c r="O16" s="3"/>
+      <c r="P16" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="7">
         <v>0</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="13">
+      <c r="E17" s="3"/>
+      <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="14">
+      <c r="G17" s="3"/>
+      <c r="H17" s="8">
         <v>2</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="7">
         <v>0</v>
       </c>
-      <c r="M17" s="9"/>
-      <c r="N17" s="13">
+      <c r="M17" s="3"/>
+      <c r="N17" s="7">
         <v>1</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="14">
+      <c r="O17" s="3"/>
+      <c r="P17" s="8">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uploaded hte daily files
</commit_message>
<xml_diff>
--- a/files/Matières/EPS/T1/Récup des temps.xlsx
+++ b/files/Matières/EPS/T1/Récup des temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\EPS\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A32C0A3-ABAE-4B38-8145-01233A24F352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF22C79-7276-470F-A360-F5E8AA37AF07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{57035DCE-7893-496B-BF95-86A9CDE9C012}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Date du 2*800:</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Temps Garçon</t>
+  </si>
+  <si>
+    <t>Lien du tableau: https://bit.ly/3qV0jh4</t>
+  </si>
+  <si>
+    <t>Serveur Discord: https://discord.gg/kATGfaDhuu</t>
   </si>
 </sst>
 </file>
@@ -589,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5872A0-D558-4440-BC29-71C64DDB7472}">
-  <dimension ref="C1:P17"/>
+  <dimension ref="C1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -609,7 +615,7 @@
     <col min="13" max="13" width="1.73046875" customWidth="1"/>
     <col min="14" max="14" width="4.1328125" customWidth="1"/>
     <col min="15" max="15" width="1.46484375" customWidth="1"/>
-    <col min="16" max="16" width="6.9296875" customWidth="1"/>
+    <col min="16" max="16" width="7.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -955,6 +961,16 @@
       <c r="O17" s="3"/>
       <c r="P17" s="8">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploaded and updated a few files
</commit_message>
<xml_diff>
--- a/files/Matières/EPS/T1/Récup des temps.xlsx
+++ b/files/Matières/EPS/T1/Récup des temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\EPS\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF22C79-7276-470F-A360-F5E8AA37AF07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B3CB2F-52BA-49E1-978A-A696CB02AD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{57035DCE-7893-496B-BF95-86A9CDE9C012}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Date du 2*800:</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Serveur Discord: https://discord.gg/kATGfaDhuu</t>
+  </si>
+  <si>
+    <t>Pour les temps, il n'y a aucun besoin de faire de calculs. Il vous suffit de vous rappeler du temps donné par le professeur à chaque tour de piste.</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5872A0-D558-4440-BC29-71C64DDB7472}">
-  <dimension ref="C1:P21"/>
+  <dimension ref="C1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -963,13 +966,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C20" t="s">
-        <v>18</v>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded the holiday files
</commit_message>
<xml_diff>
--- a/files/Matières/EPS/T1/Récup des temps.xlsx
+++ b/files/Matières/EPS/T1/Récup des temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\EPS\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B3CB2F-52BA-49E1-978A-A696CB02AD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C61474-B675-40D3-8ED3-A2B78699D0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{57035DCE-7893-496B-BF95-86A9CDE9C012}"/>
   </bookViews>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5872A0-D558-4440-BC29-71C64DDB7472}">
   <dimension ref="C1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>